<commit_message>
Added the risk of 'inadequate testing'
</commit_message>
<xml_diff>
--- a/Risk managment.xlsx
+++ b/Risk managment.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Cause</t>
   </si>
@@ -51,13 +51,22 @@
     <t>Can result in parts of the project not being completed on time. Can also result in me not receiving the help I need from the trainers.</t>
   </si>
   <si>
-    <t>Contracting Coronavirus</t>
-  </si>
-  <si>
     <t>This project will be carried out during a pandemic where chances of catching the virus will be extremely high</t>
   </si>
   <si>
     <t>The illness can severly impact my abilty to work.</t>
+  </si>
+  <si>
+    <t>Covid-19</t>
+  </si>
+  <si>
+    <t>Inadequate testing</t>
+  </si>
+  <si>
+    <t>This may be due to insufficient unite testing or not closly adhering to the TDD methodology</t>
+  </si>
+  <si>
+    <t>This will result is some aspects of the software behaving unexpectadly.</t>
   </si>
 </sst>
 </file>
@@ -404,8 +413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,21 +470,28 @@
     </row>
     <row r="9" spans="3:13" ht="75" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="3:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="1"/>
-      <c r="E10" s="1"/>
+    <row r="10" spans="3:13" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="11" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>

</xml_diff>